<commit_message>
Initial very rough experiments
</commit_message>
<xml_diff>
--- a/sample-data/first-fleet-maps.xlsx
+++ b/sample-data/first-fleet-maps.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24880" windowHeight="15600"/>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="173">
-  <si>
-    <t>itemid</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="175">
   <si>
     <t>title</t>
   </si>
@@ -31,9 +28,6 @@
     <t>caption</t>
   </si>
   <si>
-    <t>creator</t>
-  </si>
-  <si>
     <t>albumnumber</t>
   </si>
   <si>
@@ -539,6 +533,18 @@
   </si>
   <si>
     <t>Still Image</t>
+  </si>
+  <si>
+    <t>dc:title</t>
+  </si>
+  <si>
+    <t>dc:type</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>&gt;dc:creator</t>
   </si>
 </sst>
 </file>
@@ -960,7 +966,7 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -975,60 +981,60 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>173</v>
       </c>
       <c r="C1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B2">
         <v>902810</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F2">
         <v>903932</v>
@@ -1037,777 +1043,777 @@
         <v>1788</v>
       </c>
       <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>15</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>16</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>17</v>
-      </c>
-      <c r="L2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B3">
         <v>480022</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F3">
         <v>862353</v>
       </c>
       <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
         <v>23</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>24</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>25</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>26</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>27</v>
-      </c>
-      <c r="L3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B4">
         <v>480023</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F4">
         <v>862353</v>
       </c>
       <c r="G4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" t="s">
         <v>23</v>
       </c>
-      <c r="H4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" t="s">
-        <v>25</v>
-      </c>
       <c r="J4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" t="s">
         <v>31</v>
       </c>
-      <c r="K4" t="s">
+      <c r="M4" t="s">
         <v>32</v>
-      </c>
-      <c r="L4" t="s">
-        <v>33</v>
-      </c>
-      <c r="M4" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B5">
         <v>480024</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F5">
         <v>862353</v>
       </c>
       <c r="G5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" t="s">
         <v>23</v>
       </c>
-      <c r="H5" t="s">
-        <v>24</v>
-      </c>
-      <c r="I5" t="s">
-        <v>25</v>
-      </c>
       <c r="J5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5" t="s">
         <v>36</v>
       </c>
-      <c r="K5" t="s">
+      <c r="M5" t="s">
         <v>37</v>
-      </c>
-      <c r="L5" t="s">
-        <v>38</v>
-      </c>
-      <c r="M5" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B6">
         <v>480025</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F6">
         <v>862353</v>
       </c>
       <c r="G6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" t="s">
         <v>23</v>
       </c>
-      <c r="H6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I6" t="s">
-        <v>25</v>
-      </c>
       <c r="J6" t="s">
+        <v>39</v>
+      </c>
+      <c r="K6" t="s">
+        <v>40</v>
+      </c>
+      <c r="L6" t="s">
         <v>41</v>
       </c>
-      <c r="K6" t="s">
+      <c r="M6" t="s">
         <v>42</v>
-      </c>
-      <c r="L6" t="s">
-        <v>43</v>
-      </c>
-      <c r="M6" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B7">
         <v>480026</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F7">
         <v>862353</v>
       </c>
       <c r="G7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" t="s">
         <v>23</v>
       </c>
-      <c r="H7" t="s">
-        <v>24</v>
-      </c>
-      <c r="I7" t="s">
-        <v>25</v>
-      </c>
       <c r="J7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L7" t="s">
         <v>46</v>
       </c>
-      <c r="K7" t="s">
+      <c r="M7" t="s">
         <v>47</v>
-      </c>
-      <c r="L7" t="s">
-        <v>48</v>
-      </c>
-      <c r="M7" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B8">
         <v>480027</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F8">
         <v>862353</v>
       </c>
       <c r="G8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" t="s">
         <v>23</v>
       </c>
-      <c r="H8" t="s">
-        <v>24</v>
-      </c>
-      <c r="I8" t="s">
-        <v>25</v>
-      </c>
       <c r="J8" t="s">
+        <v>49</v>
+      </c>
+      <c r="K8" t="s">
+        <v>50</v>
+      </c>
+      <c r="L8" t="s">
         <v>51</v>
       </c>
-      <c r="K8" t="s">
+      <c r="M8" t="s">
         <v>52</v>
-      </c>
-      <c r="L8" t="s">
-        <v>53</v>
-      </c>
-      <c r="M8" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B9">
         <v>480028</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E9" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F9">
         <v>862353</v>
       </c>
       <c r="G9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I9" t="s">
         <v>23</v>
       </c>
-      <c r="H9" t="s">
-        <v>24</v>
-      </c>
-      <c r="I9" t="s">
-        <v>25</v>
-      </c>
       <c r="J9" t="s">
+        <v>54</v>
+      </c>
+      <c r="K9" t="s">
+        <v>55</v>
+      </c>
+      <c r="L9" t="s">
         <v>56</v>
       </c>
-      <c r="K9" t="s">
+      <c r="M9" t="s">
         <v>57</v>
-      </c>
-      <c r="L9" t="s">
-        <v>58</v>
-      </c>
-      <c r="M9" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B10">
         <v>480029</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E10" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F10">
         <v>862353</v>
       </c>
       <c r="G10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" t="s">
         <v>23</v>
       </c>
-      <c r="H10" t="s">
-        <v>24</v>
-      </c>
-      <c r="I10" t="s">
-        <v>25</v>
-      </c>
       <c r="J10" t="s">
+        <v>59</v>
+      </c>
+      <c r="K10" t="s">
+        <v>60</v>
+      </c>
+      <c r="L10" t="s">
         <v>61</v>
       </c>
-      <c r="K10" t="s">
+      <c r="M10" t="s">
         <v>62</v>
-      </c>
-      <c r="L10" t="s">
-        <v>63</v>
-      </c>
-      <c r="M10" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B11">
         <v>480030</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E11" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F11">
         <v>862353</v>
       </c>
       <c r="G11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" t="s">
         <v>23</v>
       </c>
-      <c r="H11" t="s">
-        <v>24</v>
-      </c>
-      <c r="I11" t="s">
-        <v>25</v>
-      </c>
       <c r="J11" t="s">
+        <v>64</v>
+      </c>
+      <c r="K11" t="s">
+        <v>65</v>
+      </c>
+      <c r="L11" t="s">
         <v>66</v>
       </c>
-      <c r="K11" t="s">
+      <c r="M11" t="s">
         <v>67</v>
-      </c>
-      <c r="L11" t="s">
-        <v>68</v>
-      </c>
-      <c r="M11" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B12">
         <v>480031</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F12">
         <v>862353</v>
       </c>
       <c r="G12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" t="s">
         <v>23</v>
       </c>
-      <c r="H12" t="s">
-        <v>24</v>
-      </c>
-      <c r="I12" t="s">
-        <v>25</v>
-      </c>
       <c r="J12" t="s">
+        <v>69</v>
+      </c>
+      <c r="K12" t="s">
+        <v>70</v>
+      </c>
+      <c r="L12" t="s">
         <v>71</v>
       </c>
-      <c r="K12" t="s">
+      <c r="M12" t="s">
         <v>72</v>
-      </c>
-      <c r="L12" t="s">
-        <v>73</v>
-      </c>
-      <c r="M12" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B13">
         <v>480032</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E13" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F13">
         <v>862353</v>
       </c>
       <c r="G13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" t="s">
         <v>23</v>
       </c>
-      <c r="H13" t="s">
-        <v>24</v>
-      </c>
-      <c r="I13" t="s">
-        <v>25</v>
-      </c>
       <c r="J13" t="s">
+        <v>74</v>
+      </c>
+      <c r="K13" t="s">
+        <v>75</v>
+      </c>
+      <c r="L13" t="s">
         <v>76</v>
       </c>
-      <c r="K13" t="s">
+      <c r="M13" t="s">
         <v>77</v>
-      </c>
-      <c r="L13" t="s">
-        <v>78</v>
-      </c>
-      <c r="M13" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B14">
         <v>480033</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E14" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F14">
         <v>862353</v>
       </c>
       <c r="G14" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" t="s">
         <v>23</v>
       </c>
-      <c r="H14" t="s">
-        <v>24</v>
-      </c>
-      <c r="I14" t="s">
-        <v>25</v>
-      </c>
       <c r="J14" t="s">
+        <v>79</v>
+      </c>
+      <c r="K14" t="s">
+        <v>80</v>
+      </c>
+      <c r="L14" t="s">
         <v>81</v>
       </c>
-      <c r="K14" t="s">
+      <c r="M14" t="s">
         <v>82</v>
-      </c>
-      <c r="L14" t="s">
-        <v>83</v>
-      </c>
-      <c r="M14" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B15">
         <v>480034</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E15" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F15">
         <v>862353</v>
       </c>
       <c r="G15" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" t="s">
         <v>23</v>
       </c>
-      <c r="H15" t="s">
-        <v>24</v>
-      </c>
-      <c r="I15" t="s">
-        <v>25</v>
-      </c>
       <c r="J15" t="s">
+        <v>84</v>
+      </c>
+      <c r="K15" t="s">
+        <v>85</v>
+      </c>
+      <c r="L15" t="s">
         <v>86</v>
       </c>
-      <c r="K15" t="s">
+      <c r="M15" t="s">
         <v>87</v>
-      </c>
-      <c r="L15" t="s">
-        <v>88</v>
-      </c>
-      <c r="M15" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:13">
       <c r="A16" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B16">
         <v>887137</v>
       </c>
       <c r="C16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E16" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F16">
         <v>889870</v>
       </c>
       <c r="G16" t="s">
+        <v>90</v>
+      </c>
+      <c r="H16" t="s">
+        <v>91</v>
+      </c>
+      <c r="I16" t="s">
         <v>92</v>
       </c>
-      <c r="H16" t="s">
+      <c r="J16" t="s">
         <v>93</v>
       </c>
-      <c r="I16" t="s">
+      <c r="K16" t="s">
         <v>94</v>
       </c>
-      <c r="J16" t="s">
+      <c r="L16" t="s">
         <v>95</v>
       </c>
-      <c r="K16" t="s">
+      <c r="M16" t="s">
         <v>96</v>
-      </c>
-      <c r="L16" t="s">
-        <v>97</v>
-      </c>
-      <c r="M16" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B17">
         <v>887141</v>
       </c>
       <c r="C17" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D17" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E17" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F17">
         <v>889972</v>
       </c>
       <c r="G17" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H17" t="s">
+        <v>98</v>
+      </c>
+      <c r="I17" t="s">
+        <v>99</v>
+      </c>
+      <c r="J17" t="s">
         <v>100</v>
       </c>
-      <c r="I17" t="s">
+      <c r="K17" t="s">
         <v>101</v>
       </c>
-      <c r="J17" t="s">
+      <c r="L17" t="s">
         <v>102</v>
       </c>
-      <c r="K17" t="s">
+      <c r="M17" t="s">
         <v>103</v>
-      </c>
-      <c r="L17" t="s">
-        <v>104</v>
-      </c>
-      <c r="M17" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:13">
       <c r="A18" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B18">
         <v>902815</v>
       </c>
       <c r="C18" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D18" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E18" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F18">
         <v>903940</v>
       </c>
       <c r="G18" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H18" t="s">
+        <v>105</v>
+      </c>
+      <c r="I18" t="s">
+        <v>106</v>
+      </c>
+      <c r="J18" t="s">
         <v>107</v>
       </c>
-      <c r="I18" t="s">
+      <c r="K18" t="s">
         <v>108</v>
       </c>
-      <c r="J18" t="s">
+      <c r="L18" t="s">
         <v>109</v>
       </c>
-      <c r="K18" t="s">
+      <c r="M18" t="s">
         <v>110</v>
-      </c>
-      <c r="L18" t="s">
-        <v>111</v>
-      </c>
-      <c r="M18" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:13">
       <c r="A19" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B19">
         <v>903891</v>
       </c>
       <c r="C19" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D19" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E19" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F19">
         <v>913701</v>
       </c>
       <c r="G19" t="s">
+        <v>113</v>
+      </c>
+      <c r="H19" t="s">
+        <v>114</v>
+      </c>
+      <c r="I19" t="s">
         <v>115</v>
       </c>
-      <c r="H19" t="s">
+      <c r="J19" t="s">
         <v>116</v>
       </c>
-      <c r="I19" t="s">
+      <c r="K19" t="s">
         <v>117</v>
       </c>
-      <c r="J19" t="s">
+      <c r="L19" t="s">
         <v>118</v>
       </c>
-      <c r="K19" t="s">
+      <c r="M19" t="s">
         <v>119</v>
-      </c>
-      <c r="L19" t="s">
-        <v>120</v>
-      </c>
-      <c r="M19" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:13">
       <c r="A20" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B20">
         <v>903892</v>
       </c>
       <c r="C20" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D20" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E20" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F20">
         <v>913700</v>
       </c>
       <c r="G20" t="s">
+        <v>122</v>
+      </c>
+      <c r="H20" t="s">
+        <v>123</v>
+      </c>
+      <c r="I20" t="s">
         <v>124</v>
       </c>
-      <c r="H20" t="s">
+      <c r="J20" t="s">
         <v>125</v>
       </c>
-      <c r="I20" t="s">
+      <c r="K20" t="s">
         <v>126</v>
       </c>
-      <c r="J20" t="s">
+      <c r="L20" t="s">
         <v>127</v>
       </c>
-      <c r="K20" t="s">
+      <c r="M20" t="s">
         <v>128</v>
-      </c>
-      <c r="L20" t="s">
-        <v>129</v>
-      </c>
-      <c r="M20" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="21" spans="1:13">
       <c r="A21" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B21">
         <v>903896</v>
       </c>
       <c r="C21" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D21" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E21" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F21">
         <v>913724</v>
@@ -1816,80 +1822,80 @@
         <v>1791</v>
       </c>
       <c r="H21" t="s">
+        <v>130</v>
+      </c>
+      <c r="I21" t="s">
+        <v>131</v>
+      </c>
+      <c r="J21" t="s">
         <v>132</v>
       </c>
-      <c r="I21" t="s">
+      <c r="K21" t="s">
         <v>133</v>
       </c>
-      <c r="J21" t="s">
+      <c r="L21" t="s">
         <v>134</v>
       </c>
-      <c r="K21" t="s">
+      <c r="M21" t="s">
         <v>135</v>
-      </c>
-      <c r="L21" t="s">
-        <v>136</v>
-      </c>
-      <c r="M21" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="22" spans="1:13">
       <c r="A22" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B22">
         <v>909019</v>
       </c>
       <c r="C22" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D22" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E22" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F22">
         <v>910700</v>
       </c>
       <c r="G22" t="s">
+        <v>137</v>
+      </c>
+      <c r="H22" t="s">
+        <v>138</v>
+      </c>
+      <c r="I22" t="s">
         <v>139</v>
       </c>
-      <c r="H22" t="s">
+      <c r="J22" t="s">
         <v>140</v>
       </c>
-      <c r="I22" t="s">
+      <c r="K22" t="s">
         <v>141</v>
       </c>
-      <c r="J22" t="s">
+      <c r="L22" t="s">
         <v>142</v>
       </c>
-      <c r="K22" t="s">
+      <c r="M22" t="s">
         <v>143</v>
-      </c>
-      <c r="L22" t="s">
-        <v>144</v>
-      </c>
-      <c r="M22" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="23" spans="1:13">
       <c r="A23" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B23">
         <v>478053</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D23" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E23" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F23">
         <v>861495</v>
@@ -1898,39 +1904,39 @@
         <v>1789</v>
       </c>
       <c r="H23" t="s">
+        <v>147</v>
+      </c>
+      <c r="I23" t="s">
+        <v>148</v>
+      </c>
+      <c r="J23" t="s">
         <v>149</v>
       </c>
-      <c r="I23" t="s">
+      <c r="K23" t="s">
         <v>150</v>
       </c>
-      <c r="J23" t="s">
+      <c r="L23" t="s">
         <v>151</v>
       </c>
-      <c r="K23" t="s">
+      <c r="M23" t="s">
         <v>152</v>
-      </c>
-      <c r="L23" t="s">
-        <v>153</v>
-      </c>
-      <c r="M23" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="24" spans="1:13">
       <c r="A24" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B24">
         <v>902821</v>
       </c>
       <c r="C24" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D24" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E24" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F24">
         <v>903944</v>
@@ -1939,22 +1945,22 @@
         <v>1797</v>
       </c>
       <c r="H24" t="s">
+        <v>156</v>
+      </c>
+      <c r="I24" t="s">
+        <v>157</v>
+      </c>
+      <c r="J24" t="s">
         <v>158</v>
       </c>
-      <c r="I24" t="s">
+      <c r="K24" t="s">
         <v>159</v>
       </c>
-      <c r="J24" t="s">
+      <c r="L24" t="s">
         <v>160</v>
       </c>
-      <c r="K24" t="s">
+      <c r="M24" t="s">
         <v>161</v>
-      </c>
-      <c r="L24" t="s">
-        <v>162</v>
-      </c>
-      <c r="M24" t="s">
-        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -1984,30 +1990,30 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
       <c r="D1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E2">
         <v>1818</v>
@@ -2015,13 +2021,13 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D3">
         <v>1758</v>
@@ -2032,24 +2038,24 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>